<commit_message>
added sound and movement
</commit_message>
<xml_diff>
--- a/motor_test_5_all_motors/Mecanum-Wheel-Direction-Map.xlsx
+++ b/motor_test_5_all_motors/Mecanum-Wheel-Direction-Map.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\comp444\motor_test_5_all_motors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\comp444dev\motor_test_5_all_motors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E10CE-64AC-49E2-AD34-842E6143C8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977C2840-A4CA-4823-B944-8C473CA93AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="2835" windowWidth="16740" windowHeight="13020" xr2:uid="{6527D9AB-E244-4857-8155-696781F2A149}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{6527D9AB-E244-4857-8155-696781F2A149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="24">
   <si>
     <t>direction</t>
   </si>
@@ -93,6 +94,21 @@
   </si>
   <si>
     <t>stopped</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>FRONT_LEFT</t>
+  </si>
+  <si>
+    <t>FRONT_RIGHT</t>
+  </si>
+  <si>
+    <t>REAR_LEFT</t>
+  </si>
+  <si>
+    <t>REAR_RIGHT</t>
   </si>
 </sst>
 </file>
@@ -471,45 +487,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268725DA-1603-4351-BFC3-0CA6999AB01B}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -526,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -543,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -560,7 +576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -577,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -594,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -611,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -628,7 +644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -645,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -662,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -679,7 +695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -704,4 +720,438 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124BA0E1-2CAD-4486-99AD-D36ADEBEE1A2}">
+  <dimension ref="B3:J49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46:I49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I29" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I35" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I37" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I40" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I44" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
+      </c>
+      <c r="J46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I47" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="I48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I49" t="s">
+        <v>23</v>
+      </c>
+      <c r="J49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>